<commit_message>
change detail & map luoi dien
</commit_message>
<xml_diff>
--- a/wp-content/themes/power/templates/Bitexco.xlsx
+++ b/wp-content/themes/power/templates/Bitexco.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Xamp_74\htdocs\new_bitexco\wp-content\themes\power\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{149ACA8D-4799-4982-B8F4-A9EE15849936}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBFB988A-0B62-4FC5-8693-FD1E5CB5972E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Năm" sheetId="1" r:id="rId1"/>
@@ -647,7 +647,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="59">
   <si>
     <t>Thủy điện</t>
   </si>
@@ -728,129 +728,6 @@
   </si>
   <si>
     <t>Tổng tháng</t>
-  </si>
-  <si>
-    <t>KM1</t>
-  </si>
-  <si>
-    <t>KM2</t>
-  </si>
-  <si>
-    <t>KM3</t>
-  </si>
-  <si>
-    <t>KM4</t>
-  </si>
-  <si>
-    <t>KM5</t>
-  </si>
-  <si>
-    <t>KM6</t>
-  </si>
-  <si>
-    <t>KM7</t>
-  </si>
-  <si>
-    <t>KM8</t>
-  </si>
-  <si>
-    <t>KM9</t>
-  </si>
-  <si>
-    <t>KM10</t>
-  </si>
-  <si>
-    <t>KM11</t>
-  </si>
-  <si>
-    <t>KM12</t>
-  </si>
-  <si>
-    <t>KD2-1</t>
-  </si>
-  <si>
-    <t>KD2-2</t>
-  </si>
-  <si>
-    <t>KD2-3</t>
-  </si>
-  <si>
-    <t>KD2-4</t>
-  </si>
-  <si>
-    <t>KD2-5</t>
-  </si>
-  <si>
-    <t>KD2-6</t>
-  </si>
-  <si>
-    <t>KD2-7</t>
-  </si>
-  <si>
-    <t>KD2-8</t>
-  </si>
-  <si>
-    <t>KD2-9</t>
-  </si>
-  <si>
-    <t>KD2-10</t>
-  </si>
-  <si>
-    <t>KD2-11</t>
-  </si>
-  <si>
-    <t>KD2-12</t>
-  </si>
-  <si>
-    <t>KD2-13</t>
-  </si>
-  <si>
-    <t>KD2-14</t>
-  </si>
-  <si>
-    <t>KD2-15</t>
-  </si>
-  <si>
-    <t>KD2-16</t>
-  </si>
-  <si>
-    <t>KD2-17</t>
-  </si>
-  <si>
-    <t>KD2-19</t>
-  </si>
-  <si>
-    <t>KD2-20</t>
-  </si>
-  <si>
-    <t>KD2-21</t>
-  </si>
-  <si>
-    <t>KD2-22</t>
-  </si>
-  <si>
-    <t>KD2-23</t>
-  </si>
-  <si>
-    <t>KD2-24</t>
-  </si>
-  <si>
-    <t>KD2-25</t>
-  </si>
-  <si>
-    <t>KD2-26</t>
-  </si>
-  <si>
-    <t>KD2-27</t>
-  </si>
-  <si>
-    <t>KD2-28</t>
-  </si>
-  <si>
-    <t>KD2-18</t>
-  </si>
-  <si>
-    <t>KD2-29</t>
   </si>
   <si>
     <t>KD1-1</t>
@@ -947,9 +824,6 @@
   </si>
   <si>
     <t>KD1-32</t>
-  </si>
-  <si>
-    <t>KYEAR</t>
   </si>
 </sst>
 </file>
@@ -2138,9 +2012,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K943"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J2" sqref="J2"/>
+      <selection pane="bottomLeft" activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2149,7 +2023,7 @@
     <col min="2" max="2" width="14" customWidth="1"/>
     <col min="3" max="3" width="14" style="4" customWidth="1"/>
     <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="5" max="5" width="22.7109375" customWidth="1"/>
+    <col min="5" max="5" width="15.85546875" customWidth="1"/>
     <col min="6" max="6" width="16.42578125" customWidth="1"/>
     <col min="7" max="8" width="14.85546875" customWidth="1"/>
     <col min="9" max="9" width="14" customWidth="1"/>
@@ -2216,16 +2090,13 @@
         <v>140</v>
       </c>
       <c r="H2" s="13">
-        <f>('Tháng 1'!G33)</f>
+        <f>('Tháng 1'!H33)</f>
         <v>140</v>
       </c>
       <c r="I2" s="13">
         <f>SUM(B2:H2)</f>
         <v>34192</v>
       </c>
-      <c r="J2" t="s">
-        <v>27</v>
-      </c>
       <c r="K2" s="12"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -2234,15 +2105,15 @@
       </c>
       <c r="B3" s="13">
         <f>('Tháng 2'!B30)</f>
-        <v>506</v>
+        <v>606</v>
       </c>
       <c r="C3" s="13">
         <f>('Tháng 2'!C30)</f>
-        <v>415</v>
+        <v>505</v>
       </c>
       <c r="D3" s="13">
         <f>('Tháng 2'!D30)</f>
-        <v>505</v>
+        <v>686</v>
       </c>
       <c r="E3" s="13">
         <f>('Tháng 2'!E30)</f>
@@ -2250,22 +2121,19 @@
       </c>
       <c r="F3" s="13">
         <f>('Tháng 2'!F30)</f>
-        <v>505</v>
+        <v>701</v>
       </c>
       <c r="G3" s="13">
         <f>('Tháng 2'!G30)</f>
-        <v>410</v>
+        <v>430</v>
       </c>
       <c r="H3" s="13">
-        <f>('Tháng 2'!G30)</f>
-        <v>410</v>
+        <f>('Tháng 2'!H30)</f>
+        <v>581</v>
       </c>
       <c r="I3" s="13">
         <f t="shared" ref="I3:I13" si="0">SUM(B3:H3)</f>
-        <v>3256</v>
-      </c>
-      <c r="J3" t="s">
-        <v>28</v>
+        <v>4014</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -2303,9 +2171,6 @@
       <c r="I4" s="13">
         <f t="shared" si="0"/>
         <v>34188</v>
-      </c>
-      <c r="J4" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2323,9 +2188,6 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J5" t="s">
-        <v>30</v>
-      </c>
     </row>
     <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
@@ -2342,9 +2204,6 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J6" t="s">
-        <v>31</v>
-      </c>
     </row>
     <row r="7" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
@@ -2361,9 +2220,6 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J7" t="s">
-        <v>32</v>
-      </c>
     </row>
     <row r="8" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
@@ -2380,9 +2236,6 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J8" t="s">
-        <v>33</v>
-      </c>
     </row>
     <row r="9" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
@@ -2399,9 +2252,6 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J9" t="s">
-        <v>34</v>
-      </c>
     </row>
     <row r="10" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
@@ -2418,9 +2268,6 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J10" t="s">
-        <v>35</v>
-      </c>
     </row>
     <row r="11" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
@@ -2437,9 +2284,6 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J11" t="s">
-        <v>36</v>
-      </c>
     </row>
     <row r="12" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
@@ -2456,9 +2300,6 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J12" t="s">
-        <v>37</v>
-      </c>
     </row>
     <row r="13" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
@@ -2475,9 +2316,6 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J13" t="s">
-        <v>38</v>
-      </c>
     </row>
     <row r="14" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
@@ -2485,15 +2323,15 @@
       </c>
       <c r="B14" s="13">
         <f>SUM(B2:B13)</f>
-        <v>566</v>
+        <v>666</v>
       </c>
       <c r="C14" s="13">
         <f t="shared" ref="C14:I14" si="1">SUM(C2:C13)</f>
-        <v>975</v>
+        <v>1065</v>
       </c>
       <c r="D14" s="13">
         <f t="shared" si="1"/>
-        <v>6105</v>
+        <v>6286</v>
       </c>
       <c r="E14" s="13">
         <f t="shared" si="1"/>
@@ -2501,22 +2339,19 @@
       </c>
       <c r="F14" s="13">
         <f t="shared" si="1"/>
-        <v>6105</v>
+        <v>6301</v>
       </c>
       <c r="G14" s="13">
         <f t="shared" si="1"/>
-        <v>690</v>
+        <v>710</v>
       </c>
       <c r="H14" s="13">
         <f t="shared" ref="H14" si="2">SUM(H2:H13)</f>
-        <v>690</v>
+        <v>861</v>
       </c>
       <c r="I14" s="13">
         <f t="shared" si="1"/>
-        <v>71636</v>
-      </c>
-      <c r="J14" t="s">
-        <v>100</v>
+        <v>72394</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -9808,7 +9643,7 @@
         <v>1221</v>
       </c>
       <c r="J2" t="s">
-        <v>68</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -9841,7 +9676,7 @@
         <v>1222</v>
       </c>
       <c r="J3" t="s">
-        <v>69</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -9874,7 +9709,7 @@
         <v>1223</v>
       </c>
       <c r="J4" t="s">
-        <v>70</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -9907,7 +9742,7 @@
         <v>1224</v>
       </c>
       <c r="J5" t="s">
-        <v>71</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -9940,7 +9775,7 @@
         <v>1225</v>
       </c>
       <c r="J6" t="s">
-        <v>72</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -9973,7 +9808,7 @@
         <v>1226</v>
       </c>
       <c r="J7" t="s">
-        <v>73</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -10006,7 +9841,7 @@
         <v>1227</v>
       </c>
       <c r="J8" t="s">
-        <v>74</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -10039,7 +9874,7 @@
         <v>1228</v>
       </c>
       <c r="J9" t="s">
-        <v>75</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -10072,7 +9907,7 @@
         <v>1229</v>
       </c>
       <c r="J10" t="s">
-        <v>76</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -10105,7 +9940,7 @@
         <v>1230</v>
       </c>
       <c r="J11" t="s">
-        <v>77</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -10138,7 +9973,7 @@
         <v>1231</v>
       </c>
       <c r="J12" t="s">
-        <v>78</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -10171,7 +10006,7 @@
         <v>1232</v>
       </c>
       <c r="J13" t="s">
-        <v>79</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -10204,7 +10039,7 @@
         <v>1233</v>
       </c>
       <c r="J14" t="s">
-        <v>80</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -10237,7 +10072,7 @@
         <v>1234</v>
       </c>
       <c r="J15" t="s">
-        <v>81</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -10270,7 +10105,7 @@
         <v>1235</v>
       </c>
       <c r="J16" t="s">
-        <v>82</v>
+        <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -10303,7 +10138,7 @@
         <v>1236</v>
       </c>
       <c r="J17" t="s">
-        <v>83</v>
+        <v>42</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -10336,7 +10171,7 @@
         <v>1237</v>
       </c>
       <c r="J18" t="s">
-        <v>84</v>
+        <v>43</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -10369,7 +10204,7 @@
         <v>1238</v>
       </c>
       <c r="J19" t="s">
-        <v>85</v>
+        <v>44</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -10402,7 +10237,7 @@
         <v>1239</v>
       </c>
       <c r="J20" t="s">
-        <v>86</v>
+        <v>45</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -10435,7 +10270,7 @@
         <v>1240</v>
       </c>
       <c r="J21" t="s">
-        <v>87</v>
+        <v>46</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -10468,7 +10303,7 @@
         <v>1241</v>
       </c>
       <c r="J22" t="s">
-        <v>88</v>
+        <v>47</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -10501,7 +10336,7 @@
         <v>1242</v>
       </c>
       <c r="J23" t="s">
-        <v>89</v>
+        <v>48</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -10534,7 +10369,7 @@
         <v>1243</v>
       </c>
       <c r="J24" t="s">
-        <v>90</v>
+        <v>49</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -10567,7 +10402,7 @@
         <v>1244</v>
       </c>
       <c r="J25" t="s">
-        <v>91</v>
+        <v>50</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -10600,7 +10435,7 @@
         <v>1245</v>
       </c>
       <c r="J26" t="s">
-        <v>92</v>
+        <v>51</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -10633,7 +10468,7 @@
         <v>1246</v>
       </c>
       <c r="J27" t="s">
-        <v>93</v>
+        <v>52</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -10666,7 +10501,7 @@
         <v>1247</v>
       </c>
       <c r="J28" t="s">
-        <v>94</v>
+        <v>53</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -10699,7 +10534,7 @@
         <v>1248</v>
       </c>
       <c r="J29" t="s">
-        <v>95</v>
+        <v>54</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -10732,7 +10567,7 @@
         <v>1249</v>
       </c>
       <c r="J30" t="s">
-        <v>96</v>
+        <v>55</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -10765,7 +10600,7 @@
         <v>1250</v>
       </c>
       <c r="J31" t="s">
-        <v>97</v>
+        <v>56</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -10798,7 +10633,7 @@
         <v>1251</v>
       </c>
       <c r="J32" t="s">
-        <v>98</v>
+        <v>57</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -10837,7 +10672,7 @@
         <v>34192</v>
       </c>
       <c r="J33" t="s">
-        <v>99</v>
+        <v>58</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -18000,8 +17835,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F32B5ED5-A419-4C69-939D-BA9E3170FADB}">
   <dimension ref="A1:J941"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L24" sqref="L24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18049,10 +17884,10 @@
         <v>44958</v>
       </c>
       <c r="B2" s="6">
-        <v>1</v>
+        <v>101</v>
       </c>
       <c r="C2" s="6">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="D2" s="6">
         <v>100</v>
@@ -18070,11 +17905,8 @@
         <v>5</v>
       </c>
       <c r="I2" s="6">
-        <f>SUM(B2:H2)</f>
-        <v>321</v>
-      </c>
-      <c r="J2" t="s">
-        <v>39</v>
+        <f t="shared" ref="I2:I30" si="0">SUM(B2:H2)</f>
+        <v>511</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -18097,17 +17929,14 @@
         <v>2</v>
       </c>
       <c r="G3" s="6">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="H3" s="6">
         <v>2</v>
       </c>
       <c r="I3" s="6">
-        <f t="shared" ref="I3:I30" si="0">SUM(B3:H3)</f>
-        <v>14</v>
-      </c>
-      <c r="J3" t="s">
-        <v>40</v>
+        <f t="shared" si="0"/>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -18139,9 +17968,6 @@
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="J4" t="s">
-        <v>41</v>
-      </c>
     </row>
     <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
@@ -18172,9 +17998,6 @@
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="J5" t="s">
-        <v>42</v>
-      </c>
     </row>
     <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
@@ -18205,9 +18028,6 @@
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
-      <c r="J6" t="s">
-        <v>43</v>
-      </c>
     </row>
     <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
@@ -18238,9 +18058,6 @@
         <f t="shared" si="0"/>
         <v>42</v>
       </c>
-      <c r="J7" t="s">
-        <v>44</v>
-      </c>
     </row>
     <row r="8" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
@@ -18271,9 +18088,6 @@
         <f t="shared" si="0"/>
         <v>49</v>
       </c>
-      <c r="J8" t="s">
-        <v>45</v>
-      </c>
     </row>
     <row r="9" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
@@ -18304,9 +18118,6 @@
         <f t="shared" si="0"/>
         <v>56</v>
       </c>
-      <c r="J9" t="s">
-        <v>46</v>
-      </c>
     </row>
     <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
@@ -18337,9 +18148,6 @@
         <f t="shared" si="0"/>
         <v>63</v>
       </c>
-      <c r="J10" t="s">
-        <v>47</v>
-      </c>
     </row>
     <row r="11" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
@@ -18370,9 +18178,6 @@
         <f t="shared" si="0"/>
         <v>70</v>
       </c>
-      <c r="J11" t="s">
-        <v>48</v>
-      </c>
     </row>
     <row r="12" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
@@ -18403,9 +18208,6 @@
         <f t="shared" si="0"/>
         <v>77</v>
       </c>
-      <c r="J12" t="s">
-        <v>49</v>
-      </c>
     </row>
     <row r="13" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
@@ -18436,9 +18238,6 @@
         <f t="shared" si="0"/>
         <v>84</v>
       </c>
-      <c r="J13" t="s">
-        <v>50</v>
-      </c>
     </row>
     <row r="14" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
@@ -18469,9 +18268,6 @@
         <f t="shared" si="0"/>
         <v>91</v>
       </c>
-      <c r="J14" t="s">
-        <v>51</v>
-      </c>
     </row>
     <row r="15" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
@@ -18502,9 +18298,6 @@
         <f t="shared" si="0"/>
         <v>98</v>
       </c>
-      <c r="J15" t="s">
-        <v>52</v>
-      </c>
     </row>
     <row r="16" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
@@ -18535,11 +18328,8 @@
         <f t="shared" si="0"/>
         <v>105</v>
       </c>
-      <c r="J16" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>44973</v>
       </c>
@@ -18568,11 +18358,8 @@
         <f t="shared" si="0"/>
         <v>112</v>
       </c>
-      <c r="J17" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>44974</v>
       </c>
@@ -18601,11 +18388,8 @@
         <f t="shared" si="0"/>
         <v>119</v>
       </c>
-      <c r="J18" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>44975</v>
       </c>
@@ -18634,11 +18418,8 @@
         <f t="shared" si="0"/>
         <v>226</v>
       </c>
-      <c r="J19" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>44976</v>
       </c>
@@ -18649,7 +18430,7 @@
         <v>19</v>
       </c>
       <c r="D20" s="6">
-        <v>19</v>
+        <v>200</v>
       </c>
       <c r="E20" s="6">
         <v>19</v>
@@ -18661,17 +18442,14 @@
         <v>19</v>
       </c>
       <c r="H20" s="6">
-        <v>19</v>
+        <v>190</v>
       </c>
       <c r="I20" s="6">
         <f t="shared" si="0"/>
-        <v>133</v>
-      </c>
-      <c r="J20" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
         <v>44977</v>
       </c>
@@ -18700,11 +18478,8 @@
         <f t="shared" si="0"/>
         <v>140</v>
       </c>
-      <c r="J21" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
         <v>44978</v>
       </c>
@@ -18733,11 +18508,8 @@
         <f t="shared" si="0"/>
         <v>147</v>
       </c>
-      <c r="J22" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
         <v>44979</v>
       </c>
@@ -18766,11 +18538,8 @@
         <f t="shared" si="0"/>
         <v>154</v>
       </c>
-      <c r="J23" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
         <v>44980</v>
       </c>
@@ -18799,11 +18568,8 @@
         <f t="shared" si="0"/>
         <v>161</v>
       </c>
-      <c r="J24" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
         <v>44981</v>
       </c>
@@ -18832,11 +18598,8 @@
         <f t="shared" si="0"/>
         <v>168</v>
       </c>
-      <c r="J25" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
         <v>44982</v>
       </c>
@@ -18865,11 +18628,8 @@
         <f t="shared" si="0"/>
         <v>175</v>
       </c>
-      <c r="J26" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
         <v>44983</v>
       </c>
@@ -18886,7 +18646,7 @@
         <v>26</v>
       </c>
       <c r="F27" s="6">
-        <v>26</v>
+        <v>222</v>
       </c>
       <c r="G27" s="6">
         <v>26</v>
@@ -18896,13 +18656,10 @@
       </c>
       <c r="I27" s="6">
         <f t="shared" si="0"/>
-        <v>182</v>
-      </c>
-      <c r="J27" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
         <v>44984</v>
       </c>
@@ -18931,11 +18688,8 @@
         <f t="shared" si="0"/>
         <v>189</v>
       </c>
-      <c r="J28" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
         <v>44985</v>
       </c>
@@ -18964,25 +18718,22 @@
         <f t="shared" si="0"/>
         <v>196</v>
       </c>
-      <c r="J29" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>24</v>
       </c>
       <c r="B30" s="6">
         <f>SUM(B2:B29)</f>
-        <v>506</v>
+        <v>606</v>
       </c>
       <c r="C30" s="6">
         <f t="shared" ref="C30:H30" si="1">SUM(C2:C29)</f>
-        <v>415</v>
+        <v>505</v>
       </c>
       <c r="D30" s="6">
         <f t="shared" si="1"/>
-        <v>505</v>
+        <v>686</v>
       </c>
       <c r="E30" s="6">
         <f t="shared" si="1"/>
@@ -18990,28 +18741,25 @@
       </c>
       <c r="F30" s="6">
         <f t="shared" si="1"/>
-        <v>505</v>
+        <v>701</v>
       </c>
       <c r="G30" s="6">
         <f t="shared" si="1"/>
-        <v>410</v>
+        <v>430</v>
       </c>
       <c r="H30" s="6">
         <f t="shared" si="1"/>
-        <v>410</v>
+        <v>581</v>
       </c>
       <c r="I30" s="6">
         <f t="shared" si="0"/>
-        <v>3256</v>
-      </c>
-      <c r="J30" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>4014</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C31"/>
     </row>
-    <row r="32" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="33" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="34" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C34"/>
@@ -26165,7 +25913,7 @@
   <dimension ref="A1:J33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L34" sqref="L34"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
update fix bug 27/02
</commit_message>
<xml_diff>
--- a/wp-content/themes/power/templates/Bitexco.xlsx
+++ b/wp-content/themes/power/templates/Bitexco.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Xamp_74\htdocs\new_bitexco\wp-content\themes\power\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBFB988A-0B62-4FC5-8693-FD1E5CB5972E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61C5702D-D672-483E-8BCB-BE3BDEDACDCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Năm" sheetId="1" r:id="rId1"/>
@@ -833,7 +833,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -904,6 +904,19 @@
       <sz val="8"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -1021,7 +1034,7 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1057,10 +1070,23 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="12" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="7" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="12" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="11" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2012,9 +2038,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K943"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H8" sqref="H8"/>
+      <selection pane="bottomLeft" activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2023,336 +2049,349 @@
     <col min="2" max="2" width="14" customWidth="1"/>
     <col min="3" max="3" width="14" style="4" customWidth="1"/>
     <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="5" max="5" width="15.85546875" customWidth="1"/>
+    <col min="5" max="5" width="22.7109375" customWidth="1"/>
     <col min="6" max="6" width="16.42578125" customWidth="1"/>
     <col min="7" max="8" width="14.85546875" customWidth="1"/>
     <col min="9" max="9" width="14" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="11" customFormat="1" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="I1" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="J1" s="15" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="13">
+      <c r="B2" s="17">
         <f>('Tháng 1'!B33)</f>
         <v>32</v>
       </c>
-      <c r="C2" s="13">
+      <c r="C2" s="17">
         <f>('Tháng 1'!C33)</f>
         <v>280</v>
       </c>
-      <c r="D2" s="13">
+      <c r="D2" s="17">
         <f>('Tháng 1'!D33)</f>
         <v>2800</v>
       </c>
-      <c r="E2" s="13">
+      <c r="E2" s="17">
         <f>('Tháng 1'!E33)</f>
         <v>28000</v>
       </c>
-      <c r="F2" s="13">
+      <c r="F2" s="17">
         <f>('Tháng 1'!F33)</f>
         <v>2800</v>
       </c>
-      <c r="G2" s="13">
+      <c r="G2" s="17">
         <f>('Tháng 1'!G33)</f>
         <v>140</v>
       </c>
-      <c r="H2" s="13">
+      <c r="H2" s="17">
         <f>('Tháng 1'!H33)</f>
         <v>140</v>
       </c>
-      <c r="I2" s="13">
+      <c r="I2" s="17">
         <f>SUM(B2:H2)</f>
         <v>34192</v>
       </c>
+      <c r="J2" s="18"/>
       <c r="K2" s="12"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+    <row r="3" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="13">
+      <c r="B3" s="17">
         <f>('Tháng 2'!B30)</f>
         <v>606</v>
       </c>
-      <c r="C3" s="13">
+      <c r="C3" s="17">
         <f>('Tháng 2'!C30)</f>
         <v>505</v>
       </c>
-      <c r="D3" s="13">
+      <c r="D3" s="17">
         <f>('Tháng 2'!D30)</f>
-        <v>686</v>
-      </c>
-      <c r="E3" s="13">
+        <v>505</v>
+      </c>
+      <c r="E3" s="17">
         <f>('Tháng 2'!E30)</f>
         <v>505</v>
       </c>
-      <c r="F3" s="13">
+      <c r="F3" s="17">
         <f>('Tháng 2'!F30)</f>
-        <v>701</v>
-      </c>
-      <c r="G3" s="13">
+        <v>505</v>
+      </c>
+      <c r="G3" s="17">
         <f>('Tháng 2'!G30)</f>
         <v>430</v>
       </c>
-      <c r="H3" s="13">
+      <c r="H3" s="17">
         <f>('Tháng 2'!H30)</f>
-        <v>581</v>
-      </c>
-      <c r="I3" s="13">
+        <v>410</v>
+      </c>
+      <c r="I3" s="17">
         <f t="shared" ref="I3:I13" si="0">SUM(B3:H3)</f>
-        <v>4014</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+        <v>3466</v>
+      </c>
+      <c r="J3" s="18"/>
+    </row>
+    <row r="4" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="13">
+      <c r="B4" s="17">
         <f>('Tháng 3'!B33)</f>
         <v>28</v>
       </c>
-      <c r="C4" s="13">
+      <c r="C4" s="17">
         <f>('Tháng 3'!C33)</f>
         <v>280</v>
       </c>
-      <c r="D4" s="13">
+      <c r="D4" s="17">
         <f>('Tháng 3'!D33)</f>
         <v>2800</v>
       </c>
-      <c r="E4" s="13">
+      <c r="E4" s="17">
         <f>('Tháng 3'!E33)</f>
         <v>28000</v>
       </c>
-      <c r="F4" s="13">
+      <c r="F4" s="17">
         <f>('Tháng 3'!F33)</f>
         <v>2800</v>
       </c>
-      <c r="G4" s="13">
+      <c r="G4" s="17">
         <f>('Tháng 3'!G33)</f>
         <v>140</v>
       </c>
-      <c r="H4" s="13">
+      <c r="H4" s="17">
         <f>('Tháng 3'!H33)</f>
         <v>140</v>
       </c>
-      <c r="I4" s="13">
+      <c r="I4" s="17">
         <f t="shared" si="0"/>
         <v>34188</v>
       </c>
+      <c r="J4" s="18"/>
     </row>
     <row r="5" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="13"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13">
+      <c r="B5" s="17"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="17"/>
+      <c r="I5" s="17">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="J5" s="18"/>
     </row>
     <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="13"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="13"/>
-      <c r="I6" s="13">
+      <c r="B6" s="17"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="17">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="J6" s="18"/>
     </row>
     <row r="7" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="13"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="13"/>
-      <c r="I7" s="13">
+      <c r="B7" s="17"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="17"/>
+      <c r="I7" s="17">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="J7" s="18"/>
     </row>
     <row r="8" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="13"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="13"/>
-      <c r="I8" s="13">
+      <c r="B8" s="17"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="17"/>
+      <c r="I8" s="17">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="J8" s="18"/>
     </row>
     <row r="9" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="13"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="13"/>
-      <c r="I9" s="13">
+      <c r="B9" s="17"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="17">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="J9" s="18"/>
     </row>
     <row r="10" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="13"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="13">
+      <c r="B10" s="17"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="17">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="J10" s="18"/>
     </row>
     <row r="11" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="13"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
-      <c r="H11" s="13"/>
-      <c r="I11" s="13">
+      <c r="B11" s="17"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="17"/>
+      <c r="I11" s="17">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="J11" s="18"/>
     </row>
     <row r="12" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="13"/>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
-      <c r="H12" s="13"/>
-      <c r="I12" s="13">
+      <c r="B12" s="17"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="17"/>
+      <c r="G12" s="17"/>
+      <c r="H12" s="17"/>
+      <c r="I12" s="17">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="J12" s="18"/>
     </row>
     <row r="13" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="13"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
-      <c r="H13" s="13"/>
-      <c r="I13" s="13">
+      <c r="B13" s="17"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="17"/>
+      <c r="H13" s="17"/>
+      <c r="I13" s="17">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="J13" s="18"/>
     </row>
     <row r="14" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="14" t="s">
+      <c r="A14" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="13">
+      <c r="B14" s="17">
         <f>SUM(B2:B13)</f>
         <v>666</v>
       </c>
-      <c r="C14" s="13">
+      <c r="C14" s="17">
         <f t="shared" ref="C14:I14" si="1">SUM(C2:C13)</f>
         <v>1065</v>
       </c>
-      <c r="D14" s="13">
+      <c r="D14" s="17">
         <f t="shared" si="1"/>
-        <v>6286</v>
-      </c>
-      <c r="E14" s="13">
+        <v>6105</v>
+      </c>
+      <c r="E14" s="17">
         <f t="shared" si="1"/>
         <v>56505</v>
       </c>
-      <c r="F14" s="13">
+      <c r="F14" s="17">
         <f t="shared" si="1"/>
-        <v>6301</v>
-      </c>
-      <c r="G14" s="13">
+        <v>6105</v>
+      </c>
+      <c r="G14" s="17">
         <f t="shared" si="1"/>
         <v>710</v>
       </c>
-      <c r="H14" s="13">
+      <c r="H14" s="17">
         <f t="shared" ref="H14" si="2">SUM(H2:H13)</f>
-        <v>861</v>
-      </c>
-      <c r="I14" s="13">
+        <v>690</v>
+      </c>
+      <c r="I14" s="17">
         <f t="shared" si="1"/>
-        <v>72394</v>
-      </c>
+        <v>71846</v>
+      </c>
+      <c r="J14" s="18"/>
     </row>
     <row r="15" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C15"/>
@@ -17835,8 +17874,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F32B5ED5-A419-4C69-939D-BA9E3170FADB}">
   <dimension ref="A1:J941"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18430,7 +18469,7 @@
         <v>19</v>
       </c>
       <c r="D20" s="6">
-        <v>200</v>
+        <v>19</v>
       </c>
       <c r="E20" s="6">
         <v>19</v>
@@ -18442,11 +18481,11 @@
         <v>19</v>
       </c>
       <c r="H20" s="6">
-        <v>190</v>
+        <v>19</v>
       </c>
       <c r="I20" s="6">
         <f t="shared" si="0"/>
-        <v>485</v>
+        <v>133</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -18646,7 +18685,7 @@
         <v>26</v>
       </c>
       <c r="F27" s="6">
-        <v>222</v>
+        <v>26</v>
       </c>
       <c r="G27" s="6">
         <v>26</v>
@@ -18656,7 +18695,7 @@
       </c>
       <c r="I27" s="6">
         <f t="shared" si="0"/>
-        <v>378</v>
+        <v>182</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -18733,7 +18772,7 @@
       </c>
       <c r="D30" s="6">
         <f t="shared" si="1"/>
-        <v>686</v>
+        <v>505</v>
       </c>
       <c r="E30" s="6">
         <f t="shared" si="1"/>
@@ -18741,7 +18780,7 @@
       </c>
       <c r="F30" s="6">
         <f t="shared" si="1"/>
-        <v>701</v>
+        <v>505</v>
       </c>
       <c r="G30" s="6">
         <f t="shared" si="1"/>
@@ -18749,11 +18788,11 @@
       </c>
       <c r="H30" s="6">
         <f t="shared" si="1"/>
-        <v>581</v>
+        <v>410</v>
       </c>
       <c r="I30" s="6">
         <f t="shared" si="0"/>
-        <v>4014</v>
+        <v>3466</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>